<commit_message>
add measuremeent for today
</commit_message>
<xml_diff>
--- a/Measurements/027 fender rubber/measurement.xlsx
+++ b/Measurements/027 fender rubber/measurement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoe\Meng\solidworks\Measurements\027 fender rubber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF70B2D5-8618-46E7-ABA4-0901CE3CA8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069A4FB5-78FB-43CC-AACD-4E5730B8CBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Measuring Instrument Verification Record</t>
   </si>
@@ -50,14 +50,83 @@
     <t>location</t>
   </si>
   <si>
-    <t>cus_sampl</t>
+    <t>80-85</t>
+  </si>
+  <si>
+    <t>cus_smpl1</t>
+  </si>
+  <si>
+    <t>cus_smpl2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ven_smpl1</t>
+  </si>
+  <si>
+    <t>ven_smpl2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ven_smpl3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ven_smpl4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ven_smpl5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ven_smpl6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ven_smpl7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ven_smpl8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ven_smpl9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ven_smpl10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  70-85</t>
+  </si>
+  <si>
+    <t>87 - 83</t>
+  </si>
+  <si>
+    <t>88 - 83</t>
+  </si>
+  <si>
+    <t>89 - 83</t>
+  </si>
+  <si>
+    <t>90 - 83</t>
+  </si>
+  <si>
+    <t>91 - 83</t>
+  </si>
+  <si>
+    <t>92 - 83</t>
+  </si>
+  <si>
+    <t>93 - 83</t>
+  </si>
+  <si>
+    <t>94 - 83</t>
+  </si>
+  <si>
+    <t>95 - 83</t>
+  </si>
+  <si>
+    <t>96 - 83</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +166,13 @@
       <name val="Source Han Sans SC"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -402,7 +478,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -460,46 +536,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -530,7 +603,7 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>10219</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="264560"/>
@@ -589,7 +662,7 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>47649</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="342786"/>
@@ -648,7 +721,7 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>68706</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="342786"/>
@@ -707,7 +780,7 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>37290</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="342786"/>
@@ -766,7 +839,7 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>30940</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="342786"/>
@@ -884,7 +957,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>275056</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="342786"/>
@@ -943,7 +1016,7 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>234449</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="342786"/>
@@ -1002,7 +1075,7 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>94582</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="342786"/>
@@ -1061,7 +1134,7 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>56482</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="342786"/>
@@ -1120,7 +1193,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>49631</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="342786"/>
@@ -1436,36 +1509,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B969305-DC31-4967-BE1B-70216355D71C}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
     <col min="2" max="3" width="9.7109375" style="11" customWidth="1"/>
     <col min="4" max="13" width="9.7109375" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:16" ht="26.45" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1508,207 +1581,233 @@
     </row>
     <row r="4" spans="1:16" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="15">
-        <v>1</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="27"/>
+      <c r="A5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="25"/>
     </row>
     <row r="6" spans="1:16" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="15">
-        <v>2</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="27"/>
+      <c r="A6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="25"/>
     </row>
     <row r="7" spans="1:16" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="15">
-        <v>3</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="27"/>
+      <c r="A7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="25"/>
     </row>
     <row r="8" spans="1:16" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="15">
-        <v>4</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="24"/>
+      <c r="A8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="22"/>
     </row>
     <row r="9" spans="1:16" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="15">
-        <v>5</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="27"/>
+      <c r="A9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="25"/>
     </row>
     <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="15">
-        <v>6</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="27"/>
+      <c r="A10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="25"/>
     </row>
     <row r="11" spans="1:16" ht="19.5" customHeight="1">
-      <c r="A11" s="15">
-        <v>7</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="27"/>
+      <c r="A11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="25"/>
     </row>
     <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="15">
-        <v>8</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="24"/>
+      <c r="A12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="22"/>
     </row>
     <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="15">
-        <v>9</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="27"/>
-    </row>
-    <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="A14" s="18">
-        <v>10</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="32"/>
-    </row>
-    <row r="15" spans="1:16" ht="20.100000000000001" customHeight="1" thickTop="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-    </row>
-    <row r="16" spans="1:16" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="23"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="25"/>
+    </row>
+    <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="25"/>
+    </row>
+    <row r="15" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="A15" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="30"/>
+    </row>
+    <row r="16" spans="1:16" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="A16" s="7"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -1738,7 +1837,7 @@
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1933,10 +2032,26 @@
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
     </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="7"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:M1"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>